<commit_message>
add new seo xlsx
</commit_message>
<xml_diff>
--- a/allPages/allPagesRU.xlsx
+++ b/allPages/allPagesRU.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="312">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,9 @@
     <t>x</t>
   </si>
   <si>
+    <t xml:space="preserve">Услуги ВЭД, доставки и растаможки грузов в Украине в городах Киев, Львов, Одесса </t>
+  </si>
+  <si>
     <t>Услуги ВЭД, доставки и растаможки грузов в Украине в городах Киев, Львов, Одесса</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t>https://t-h-logistics.com/air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Авиа доставка и авиаперевозки грузов в Украину: быстро и надежно </t>
   </si>
   <si>
     <t>Авиа доставка и авиаперевозки грузов в Украину: быстро и надежно</t>
@@ -1365,13 +1371,13 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,22 +1385,22 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,22 +1408,22 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1425,22 +1431,22 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1448,1468 +1454,1468 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F26" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F34" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G34" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E37" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F37" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F38" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G38" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G39" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E40" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F40" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G40" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F41" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G41" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B44" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E44" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F44" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G44" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F45" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G45" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E46" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F46" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G46" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E47" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F47" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G47" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E48" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F48" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G48" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B49" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C49" t="s">
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E49" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F49" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G49" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E50" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F50" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G50" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E51" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F51" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G51" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B52" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E52" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F52" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G52" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E53" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F53" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G53" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E54" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F54" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G54" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B55" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E55" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F55" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G55" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E56" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F56" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G56" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B59" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C59" t="s">
         <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F59" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G59" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B60" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C60" t="s">
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E60" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F60" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G60" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B61" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C61" t="s">
         <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E61" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F61" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G61" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B62" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C62" t="s">
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E62" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F62" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G62" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B63" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E63" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F63" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G63" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B64" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C64" t="s">
         <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E64" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F64" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G64" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B65" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C65" t="s">
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E65" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F65" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G65" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B66" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E66" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F66" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G66" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B67" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C67" t="s">
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E67" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F67" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G67" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B70" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C70" t="s">
         <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E70" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F70" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G70" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B71" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C71" t="s">
         <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E71" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F71" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="G71" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B72" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C72" t="s">
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E72" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F72" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G72" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B73" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E73" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F73" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G73" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B74" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C74" t="s">
         <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E74" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F74" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G74" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B75" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C75" t="s">
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E75" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F75" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G75" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B76" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C76" t="s">
         <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E76" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="F76" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="G76" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B77" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C77" t="s">
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E77" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F77" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="G77" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new export file
</commit_message>
<xml_diff>
--- a/allPages/allPagesRU.xlsx
+++ b/allPages/allPagesRU.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="311">
   <si>
     <t>Date</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>https://t-h-logistics.com/air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Авиа доставка и авиаперевозки грузов в Украину: быстро и надежно </t>
   </si>
   <si>
     <t>Авиа доставка и авиаперевозки грузов в Украину: быстро и надежно</t>
@@ -464,10 +461,10 @@
     <t>Стоимость Перевозки Контейнера Морем: Надежные и Конкурентоспособные Тарифы</t>
   </si>
   <si>
-    <t xml:space="preserve">Узнайте о стоимости перевозки контейнера морем. Наши конкурентоспособные тарифы обеспечивают надежную и эффективную доставку вашего груза в любую точку мира. Мы предлагаем прозрачные цены и высокое качество обслуживания для грузоперевозок морским путем. </t>
-  </si>
-  <si>
-    <t>цена морской перевозки контейнеров, тарифы на морскую перевозку, стоимость грузоперевозок морем, расценки на перевозку морским контейнером, тарифы на контейнерные перевозки</t>
+    <t>Узнайте о стоимости перевозки контейнера морем. Наши конкурентоспособные тарифы обеспечивают надежную и эффективную доставку вашего груза в любую точку мира. Мы предлагаем прозрачные цены и высокое качество обслуживания для грузоперевозок морским путем.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">цена морской перевозки контейнеров, тарифы на морскую перевозку, стоимость грузоперевозок морем, расценки на перевозку морским контейнером, тарифы на контейнерные перевозки </t>
   </si>
   <si>
     <t>https://t-h-logistics.com/container_freight_rate</t>
@@ -1440,13 +1437,13 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1454,246 +1451,246 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>40</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>44</v>
-      </c>
-      <c r="G10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
         <v>51</v>
       </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
         <v>55</v>
       </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>60</v>
-      </c>
-      <c r="G14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
         <v>63</v>
       </c>
-      <c r="E15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>64</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>66</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>68</v>
-      </c>
-      <c r="G16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
@@ -1704,321 +1701,321 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
         <v>73</v>
       </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" t="s">
         <v>74</v>
       </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>75</v>
-      </c>
-      <c r="G18" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
         <v>78</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
         <v>79</v>
       </c>
-      <c r="E19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>80</v>
-      </c>
-      <c r="G19" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
         <v>84</v>
       </c>
-      <c r="E20" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>85</v>
-      </c>
-      <c r="G20" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
         <v>87</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
         <v>88</v>
       </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
         <v>89</v>
       </c>
-      <c r="E21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>90</v>
-      </c>
-      <c r="G21" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
         <v>92</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
         <v>94</v>
       </c>
-      <c r="E22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>95</v>
-      </c>
-      <c r="G22" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
         <v>97</v>
       </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" t="s">
         <v>98</v>
       </c>
-      <c r="E23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>99</v>
-      </c>
-      <c r="G23" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
         <v>101</v>
       </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" t="s">
         <v>102</v>
       </c>
-      <c r="E24" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>103</v>
-      </c>
-      <c r="G24" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
         <v>105</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
         <v>106</v>
       </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" t="s">
         <v>107</v>
       </c>
-      <c r="E25" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>108</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
         <v>110</v>
       </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" t="s">
         <v>111</v>
       </c>
-      <c r="E26" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>112</v>
-      </c>
-      <c r="G26" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" t="s">
         <v>115</v>
       </c>
-      <c r="E27" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" t="s">
-        <v>116</v>
-      </c>
       <c r="G27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
         <v>117</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
         <v>118</v>
       </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" t="s">
         <v>119</v>
       </c>
-      <c r="E28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>120</v>
-      </c>
-      <c r="G28" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
         <v>122</v>
       </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" t="s">
         <v>123</v>
       </c>
-      <c r="E29" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>124</v>
-      </c>
-      <c r="G29" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
         <v>126</v>
       </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>127</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>128</v>
       </c>
-      <c r="F30" t="s">
-        <v>129</v>
-      </c>
       <c r="G30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
         <v>130</v>
       </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>131</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>132</v>
-      </c>
-      <c r="F31" t="s">
-        <v>133</v>
       </c>
       <c r="G31" t="s">
         <v>18</v>
@@ -2026,896 +2023,896 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
         <v>134</v>
       </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" t="s">
         <v>135</v>
       </c>
-      <c r="E32" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>136</v>
-      </c>
-      <c r="G32" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
         <v>138</v>
       </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" t="s">
         <v>139</v>
       </c>
-      <c r="E33" t="s">
-        <v>139</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>140</v>
-      </c>
-      <c r="G33" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" t="s">
         <v>142</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
         <v>143</v>
       </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" t="s">
         <v>144</v>
       </c>
-      <c r="E34" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>145</v>
-      </c>
-      <c r="G34" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
         <v>148</v>
       </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" t="s">
         <v>149</v>
       </c>
-      <c r="E37" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>150</v>
-      </c>
-      <c r="G37" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
         <v>152</v>
       </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" t="s">
         <v>153</v>
       </c>
-      <c r="E38" t="s">
-        <v>153</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>154</v>
-      </c>
-      <c r="G38" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
         <v>156</v>
       </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F39" t="s">
         <v>157</v>
       </c>
-      <c r="E39" t="s">
-        <v>157</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>158</v>
-      </c>
-      <c r="G39" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
         <v>160</v>
       </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>161</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>162</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>163</v>
-      </c>
-      <c r="G40" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" t="s">
         <v>165</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
         <v>166</v>
       </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>166</v>
+      </c>
+      <c r="F41" t="s">
         <v>167</v>
       </c>
-      <c r="E41" t="s">
-        <v>167</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>168</v>
-      </c>
-      <c r="G41" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
         <v>171</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
         <v>172</v>
       </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>173</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
+        <v>172</v>
+      </c>
+      <c r="G44" t="s">
         <v>174</v>
-      </c>
-      <c r="F44" t="s">
-        <v>173</v>
-      </c>
-      <c r="G44" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
         <v>176</v>
       </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>176</v>
+      </c>
+      <c r="F45" t="s">
         <v>177</v>
       </c>
-      <c r="E45" t="s">
-        <v>177</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>178</v>
-      </c>
-      <c r="G45" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
         <v>180</v>
       </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" t="s">
         <v>181</v>
       </c>
-      <c r="E46" t="s">
-        <v>181</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>182</v>
-      </c>
-      <c r="G46" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
         <v>184</v>
       </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>185</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>186</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>187</v>
-      </c>
-      <c r="G47" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
         <v>189</v>
       </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>189</v>
+      </c>
+      <c r="F48" t="s">
         <v>190</v>
       </c>
-      <c r="E48" t="s">
-        <v>190</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>191</v>
-      </c>
-      <c r="G48" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
         <v>193</v>
       </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>194</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>195</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>196</v>
-      </c>
-      <c r="G49" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B50" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
         <v>198</v>
       </c>
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
+        <v>198</v>
+      </c>
+      <c r="F50" t="s">
         <v>199</v>
       </c>
-      <c r="E50" t="s">
-        <v>199</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>200</v>
-      </c>
-      <c r="G50" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" t="s">
+        <v>201</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
         <v>202</v>
       </c>
-      <c r="C51" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>203</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>204</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>205</v>
-      </c>
-      <c r="G51" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
         <v>207</v>
       </c>
-      <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>208</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>209</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>210</v>
-      </c>
-      <c r="G52" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
         <v>212</v>
       </c>
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>213</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>214</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>215</v>
-      </c>
-      <c r="G53" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
         <v>217</v>
       </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
+        <v>217</v>
+      </c>
+      <c r="F54" t="s">
         <v>218</v>
       </c>
-      <c r="E54" t="s">
-        <v>218</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>219</v>
-      </c>
-      <c r="G54" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
+        <v>220</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
         <v>221</v>
       </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>222</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>223</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>224</v>
-      </c>
-      <c r="G55" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
+        <v>225</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
         <v>226</v>
       </c>
-      <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>227</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>228</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>229</v>
-      </c>
-      <c r="G56" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" t="s">
         <v>232</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
         <v>233</v>
       </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
+        <v>233</v>
+      </c>
+      <c r="F59" t="s">
         <v>234</v>
       </c>
-      <c r="E59" t="s">
-        <v>234</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>235</v>
-      </c>
-      <c r="G59" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>236</v>
+      </c>
+      <c r="B60" t="s">
         <v>237</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
         <v>238</v>
       </c>
-      <c r="C60" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>239</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>240</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>241</v>
-      </c>
-      <c r="G60" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>242</v>
+      </c>
+      <c r="B61" t="s">
         <v>243</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
         <v>244</v>
       </c>
-      <c r="C61" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
+        <v>244</v>
+      </c>
+      <c r="F61" t="s">
         <v>245</v>
       </c>
-      <c r="E61" t="s">
-        <v>245</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>246</v>
-      </c>
-      <c r="G61" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B62" t="s">
+        <v>247</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
         <v>248</v>
       </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
+        <v>248</v>
+      </c>
+      <c r="F62" t="s">
         <v>249</v>
       </c>
-      <c r="E62" t="s">
-        <v>249</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>250</v>
-      </c>
-      <c r="G62" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>251</v>
+      </c>
+      <c r="B63" t="s">
         <v>252</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
         <v>253</v>
       </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
+        <v>253</v>
+      </c>
+      <c r="F63" t="s">
         <v>254</v>
       </c>
-      <c r="E63" t="s">
-        <v>254</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>255</v>
-      </c>
-      <c r="G63" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>256</v>
+      </c>
+      <c r="B64" t="s">
         <v>257</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="s">
         <v>258</v>
       </c>
-      <c r="C64" t="s">
-        <v>10</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
+        <v>258</v>
+      </c>
+      <c r="F64" t="s">
         <v>259</v>
       </c>
-      <c r="E64" t="s">
-        <v>259</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>260</v>
-      </c>
-      <c r="G64" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B65" t="s">
+        <v>261</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
         <v>262</v>
       </c>
-      <c r="C65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
+        <v>262</v>
+      </c>
+      <c r="F65" t="s">
         <v>263</v>
       </c>
-      <c r="E65" t="s">
-        <v>263</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>264</v>
-      </c>
-      <c r="G65" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>265</v>
+      </c>
+      <c r="B66" t="s">
         <v>266</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
         <v>267</v>
       </c>
-      <c r="C66" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>268</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>269</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>270</v>
-      </c>
-      <c r="G66" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>271</v>
+      </c>
+      <c r="B67" t="s">
         <v>272</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
         <v>273</v>
       </c>
-      <c r="C67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>274</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
+        <v>274</v>
+      </c>
+      <c r="G67" t="s">
         <v>275</v>
-      </c>
-      <c r="F67" t="s">
-        <v>275</v>
-      </c>
-      <c r="G67" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>277</v>
+      </c>
+      <c r="B70" t="s">
         <v>278</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
         <v>279</v>
       </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
+        <v>279</v>
+      </c>
+      <c r="F70" t="s">
         <v>280</v>
       </c>
-      <c r="E70" t="s">
-        <v>280</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>281</v>
-      </c>
-      <c r="G70" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B71" t="s">
+        <v>282</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
         <v>283</v>
       </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
+        <v>283</v>
+      </c>
+      <c r="F71" t="s">
         <v>284</v>
       </c>
-      <c r="E71" t="s">
-        <v>284</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>285</v>
-      </c>
-      <c r="G71" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B72" t="s">
+        <v>286</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" t="s">
         <v>287</v>
       </c>
-      <c r="C72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
+        <v>287</v>
+      </c>
+      <c r="F72" t="s">
         <v>288</v>
       </c>
-      <c r="E72" t="s">
-        <v>288</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>289</v>
-      </c>
-      <c r="G72" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" t="s">
         <v>291</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" t="s">
         <v>292</v>
       </c>
-      <c r="C73" t="s">
-        <v>10</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
+        <v>292</v>
+      </c>
+      <c r="F73" t="s">
         <v>293</v>
       </c>
-      <c r="E73" t="s">
-        <v>293</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>294</v>
-      </c>
-      <c r="G73" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B74" t="s">
+        <v>295</v>
+      </c>
+      <c r="C74" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" t="s">
         <v>296</v>
       </c>
-      <c r="C74" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
+        <v>296</v>
+      </c>
+      <c r="F74" t="s">
         <v>297</v>
       </c>
-      <c r="E74" t="s">
-        <v>297</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>298</v>
-      </c>
-      <c r="G74" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B75" t="s">
+        <v>299</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" t="s">
         <v>300</v>
       </c>
-      <c r="C75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
+        <v>300</v>
+      </c>
+      <c r="F75" t="s">
         <v>301</v>
       </c>
-      <c r="E75" t="s">
-        <v>301</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>302</v>
-      </c>
-      <c r="G75" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B76" t="s">
+        <v>303</v>
+      </c>
+      <c r="C76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" t="s">
         <v>304</v>
       </c>
-      <c r="C76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
+        <v>304</v>
+      </c>
+      <c r="F76" t="s">
         <v>305</v>
       </c>
-      <c r="E76" t="s">
-        <v>305</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>306</v>
-      </c>
-      <c r="G76" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B77" t="s">
+        <v>307</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
         <v>308</v>
       </c>
-      <c r="C77" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
+        <v>308</v>
+      </c>
+      <c r="F77" t="s">
         <v>309</v>
       </c>
-      <c r="E77" t="s">
-        <v>309</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>310</v>
-      </c>
-      <c r="G77" t="s">
-        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>